<commit_message>
Update for create new website for django and preparement for odoo
Setting up a simple website under django and try to set odoo as database.
Progress Target (not done):
Potentially would set the odoo website alone to be splited or combined in django
</commit_message>
<xml_diff>
--- a/Tripeers Website Info/Tripeers Booking Information.xlsx
+++ b/Tripeers Website Info/Tripeers Booking Information.xlsx
@@ -8,35 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis Wong\Desktop\Project Assignment\WorkTest\Tripeers Website Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BC184F-E25C-4FE8-80D3-73005F9F9752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612361E8-5985-4557-BC44-49A1AB2F11A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DBAC1A7E-A25C-4361-B3A4-B7D1FB428736}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{DBAC1A7E-A25C-4361-B3A4-B7D1FB428736}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Vehicle and Location for Prices" sheetId="1" r:id="rId1"/>
+    <sheet name="Luggage Vehicle Based Info" sheetId="2" r:id="rId2"/>
+    <sheet name="Split Version" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="79">
   <si>
     <t>LOCATION</t>
   </si>
@@ -50,9 +41,6 @@
     <t>HYUNDAI STAREX</t>
   </si>
   <si>
-    <t>TOUR VAN 14 SEATER</t>
-  </si>
-  <si>
     <t>Johor Bahru City</t>
   </si>
   <si>
@@ -206,9 +194,6 @@
     <t>Hyundai Starex</t>
   </si>
   <si>
-    <t>Tour Van 14 Seater</t>
-  </si>
-  <si>
     <t>Number of Passenger</t>
   </si>
   <si>
@@ -249,13 +234,43 @@
   </si>
   <si>
     <t>29-31 inches</t>
+  </si>
+  <si>
+    <t>14 SEATER VAN</t>
+  </si>
+  <si>
+    <t>One-Way Trip</t>
+  </si>
+  <si>
+    <t>One Round Trip</t>
+  </si>
+  <si>
+    <t>Singapore = Johor Bahru DT</t>
+  </si>
+  <si>
+    <t>14 Seater Van (seat folded)</t>
+  </si>
+  <si>
+    <t>14 Seater Van (seat used)</t>
+  </si>
+  <si>
+    <t>6B+8S</t>
+  </si>
+  <si>
+    <t>4B+6S</t>
+  </si>
+  <si>
+    <t>16M</t>
+  </si>
+  <si>
+    <t>12M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,16 +299,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -345,11 +414,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -363,25 +581,231 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -620,14 +1044,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69B2DA56-397B-4590-8266-E4122B50A42C}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{69B2DA56-397B-4590-8266-E4122B50A42C}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
   <autoFilter ref="A1:E18" xr:uid="{69B2DA56-397B-4590-8266-E4122B50A42C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{45F1E561-E5B2-4571-A14D-06432A653DF2}" name="LOCATION" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{EB715064-40A6-4741-8ED7-9EFBF21D323C}" name="TOYOTA INNOVA" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E82843E1-EBA7-4EEF-B435-DDEE6EB74815}" name="TOYOTA ALPHARD" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{4676F780-B006-466F-89FA-BF6F8EF9C32C}" name="HYUNDAI STAREX" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{EF2BD2B4-89EC-48B2-A656-1BD08610B658}" name="TOUR VAN 14 SEATER" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{45F1E561-E5B2-4571-A14D-06432A653DF2}" name="LOCATION" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{EB715064-40A6-4741-8ED7-9EFBF21D323C}" name="TOYOTA INNOVA" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{E82843E1-EBA7-4EEF-B435-DDEE6EB74815}" name="TOYOTA ALPHARD" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{4676F780-B006-466F-89FA-BF6F8EF9C32C}" name="HYUNDAI STAREX" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{EF2BD2B4-89EC-48B2-A656-1BD08610B658}" name="14 SEATER VAN" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A1FA5DE-0F64-4986-AE36-721E12FEF8C8}" name="Table13" displayName="Table13" ref="A2:E19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+  <autoFilter ref="A2:E19" xr:uid="{8A1FA5DE-0F64-4986-AE36-721E12FEF8C8}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{548B4C4D-6895-4EC6-B078-1A7137EE1327}" name="LOCATION" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{94EE1907-63F5-4363-808A-1D7AF6A8A95A}" name="TOYOTA INNOVA" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{611A356F-E385-449F-9130-A9C560192209}" name="TOYOTA ALPHARD" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{DD18A41A-C408-4DC1-B84E-3AFB9561FEE7}" name="HYUNDAI STAREX" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{9FF9D2C4-AB3A-421B-8D84-8F1FF46278CD}" name="14 SEATER VAN" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -930,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D557BD4-8D31-434D-90CB-3E32458CFE8E}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F28" sqref="A20:F28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,424 +1394,307 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="8">
-        <v>5</v>
-      </c>
-      <c r="C23" s="8">
-        <v>6</v>
-      </c>
-      <c r="D23" s="8">
-        <v>5</v>
-      </c>
-      <c r="E23" s="8">
-        <v>7</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
+    <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A21:E21"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="153" orientation="portrait" r:id="rId1"/>
@@ -1381,4 +1702,532 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AD9DE3-8D50-4729-B35A-AEE193CC2621}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="A1:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="21">
+        <v>5</v>
+      </c>
+      <c r="C3" s="21">
+        <v>6</v>
+      </c>
+      <c r="D3" s="21">
+        <v>5</v>
+      </c>
+      <c r="E3" s="21">
+        <v>7</v>
+      </c>
+      <c r="F3" s="21">
+        <v>10</v>
+      </c>
+      <c r="G3" s="21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39A94AC-F076-417C-A4EA-1B7EB12812B7}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K3" sqref="G1:K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="31.42578125" style="6" customWidth="1"/>
+    <col min="7" max="11" width="27.7109375" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="G1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update the current status for projects
1. Odoo vs django in worktest (sarawakgameproduction, FISHMASTERS)
2. Laravel and php learning and improvise. (sarawak_logistic)
3. Others, Prioritised:
a. Trippers Website Info (future changes, keeping the record)
</commit_message>
<xml_diff>
--- a/Tripeers Website Info/Tripeers Booking Information.xlsx
+++ b/Tripeers Website Info/Tripeers Booking Information.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis Wong\Desktop\Project Assignment\WorkTest\Tripeers Website Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612361E8-5985-4557-BC44-49A1AB2F11A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25397F4-6AD2-4F0E-A4DB-8E78C2674758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{DBAC1A7E-A25C-4361-B3A4-B7D1FB428736}"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle and Location for Prices" sheetId="1" r:id="rId1"/>
-    <sheet name="Luggage Vehicle Based Info" sheetId="2" r:id="rId2"/>
+    <sheet name="Luggage Vehicle Info" sheetId="2" r:id="rId2"/>
     <sheet name="Split Version" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -270,7 +270,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,14 +287,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,8 +315,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,24 +348,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -567,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -581,19 +568,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -605,13 +589,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -620,19 +604,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1706,149 +1696,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98AD9DE3-8D50-4729-B35A-AEE193CC2621}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="A1:G5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G9" sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="18">
         <v>5</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>6</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="18">
         <v>5</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="18">
         <v>7</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="18">
         <v>10</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="18">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D8" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E8" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D9" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E9" s="18" t="s">
         <v>68</v>
       </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1864,25 +1884,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="31.42578125" style="6" customWidth="1"/>
-    <col min="7" max="11" width="27.7109375" style="6" customWidth="1"/>
+    <col min="1" max="5" width="31.42578125" style="5" customWidth="1"/>
+    <col min="7" max="11" width="27.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="G1" s="15" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="G1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1900,19 +1920,19 @@
       <c r="E2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1932,19 +1952,19 @@
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="H3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>